<commit_message>
include all use property and sp500
</commit_message>
<xml_diff>
--- a/property_ratio.xlsx
+++ b/property_ratio.xlsx
@@ -12,14 +12,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$B$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$B$10</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>city</t>
   </si>
@@ -58,6 +58,15 @@
   </si>
   <si>
     <t>new_york</t>
+  </si>
+  <si>
+    <t>nasdaq 100</t>
+  </si>
+  <si>
+    <t>usa</t>
+  </si>
+  <si>
+    <t>sp500</t>
   </si>
 </sst>
 </file>
@@ -65,10 +74,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -79,6 +88,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -88,38 +120,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -179,28 +188,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -208,9 +218,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -268,181 +277,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -462,32 +471,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -540,6 +530,36 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -548,21 +568,10 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -580,31 +589,31 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -613,97 +622,97 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="34" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1201,7 +1210,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:E9">
-    <sortState ref="A2:E9">
+    <sortState ref="A1:E9">
       <sortCondition ref="E2" descending="1"/>
     </sortState>
     <extLst/>
@@ -1217,10 +1226,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="1"/>
@@ -1238,7 +1247,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1">
         <v>39.3117</v>
@@ -1286,27 +1295,46 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B8">
-        <v>14.2502</v>
+        <v>15.1352</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>14.2502</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <v>12.6292</v>
       </c>
     </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>9.4113</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:B9">
-    <sortState ref="A2:B9">
+  <autoFilter ref="A1:B10">
+    <sortState ref="A1:B10">
       <sortCondition ref="B2" descending="1"/>
     </sortState>
     <extLst/>
   </autoFilter>
+  <sortState ref="A2:B11">
+    <sortCondition ref="B2" descending="1"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>